<commit_message>
Front Panel SW added - WIP
</commit_message>
<xml_diff>
--- a/DOC/MCU_PIN_Config.xlsx
+++ b/DOC/MCU_PIN_Config.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\Source Control\SUF-Github\Electronics\suf-electronics-motor-driver\DOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\SourceControll\SUF-GitHub\Electronics\suf-electronics-motor-driver\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24960" windowHeight="10260"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PIN" sheetId="1" r:id="rId1"/>
+    <sheet name="Blocks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,8 +25,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Gömöri Zoltán</author>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gömöri Zoltán:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Control from the Machine Controller Software</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gömöri Zoltán:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Control from the Machine Controller Software</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="125">
   <si>
     <t>P0.0</t>
   </si>
@@ -361,13 +421,52 @@
   </si>
   <si>
     <t>1Wire/Analog</t>
+  </si>
+  <si>
+    <t>SPI0</t>
+  </si>
+  <si>
+    <t>SPI1</t>
+  </si>
+  <si>
+    <t>TFT</t>
+  </si>
+  <si>
+    <t>TMR0</t>
+  </si>
+  <si>
+    <t>TMR1</t>
+  </si>
+  <si>
+    <t>TMR2</t>
+  </si>
+  <si>
+    <t>SPINDLE_PWM_0</t>
+  </si>
+  <si>
+    <t>SPINDLE_PWM_1</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>TMR3</t>
+  </si>
+  <si>
+    <t>EXT/SD Card</t>
+  </si>
+  <si>
+    <t>Ext PWM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +498,19 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -445,16 +557,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -741,20 +853,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14:M17"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>44</v>
       </c>
@@ -780,7 +892,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>40</v>
       </c>
@@ -800,7 +912,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>39</v>
       </c>
@@ -820,7 +932,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>38</v>
       </c>
@@ -840,7 +952,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>37</v>
       </c>
@@ -860,7 +972,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>35</v>
       </c>
@@ -880,7 +992,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>34</v>
       </c>
@@ -900,7 +1012,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>33</v>
       </c>
@@ -920,7 +1032,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>32</v>
       </c>
@@ -935,7 +1047,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>43</v>
       </c>
@@ -958,7 +1070,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>44</v>
       </c>
@@ -981,7 +1093,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>45</v>
       </c>
@@ -1004,7 +1116,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>46</v>
       </c>
@@ -1027,7 +1139,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>47</v>
       </c>
@@ -1046,11 +1158,11 @@
       <c r="K14" t="s">
         <v>108</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="M14" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1071,7 +1183,7 @@
       </c>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1092,7 +1204,7 @@
       </c>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1113,7 +1225,7 @@
       </c>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>19</v>
       </c>
@@ -1133,7 +1245,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>20</v>
       </c>
@@ -1153,7 +1265,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>21</v>
       </c>
@@ -1169,11 +1281,11 @@
       <c r="K20" t="s">
         <v>108</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M20" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>22</v>
       </c>
@@ -1189,9 +1301,9 @@
       <c r="K21" t="s">
         <v>108</v>
       </c>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="7"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>23</v>
       </c>
@@ -1209,7 +1321,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>25</v>
       </c>
@@ -1227,7 +1339,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>26</v>
       </c>
@@ -1242,7 +1354,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>27</v>
       </c>
@@ -1257,7 +1369,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -1272,7 +1384,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1283,9 +1395,9 @@
         <v>42</v>
       </c>
       <c r="J27" s="1"/>
-      <c r="M27" s="7"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>8</v>
       </c>
@@ -1296,9 +1408,9 @@
         <v>84</v>
       </c>
       <c r="J28" s="1"/>
-      <c r="M28" s="7"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M28" s="6"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1309,9 +1421,9 @@
         <v>83</v>
       </c>
       <c r="J29" s="1"/>
-      <c r="M29" s="7"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M29" s="6"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1322,9 +1434,9 @@
         <v>82</v>
       </c>
       <c r="J30" s="1"/>
-      <c r="M30" s="7"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M30" s="6"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>11</v>
       </c>
@@ -1335,9 +1447,9 @@
         <v>81</v>
       </c>
       <c r="J31" s="1"/>
-      <c r="M31" s="7"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M31" s="6"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>13</v>
       </c>
@@ -1345,9 +1457,9 @@
         <v>30</v>
       </c>
       <c r="J32" s="1"/>
-      <c r="M32" s="7"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>14</v>
       </c>
@@ -1355,9 +1467,9 @@
         <v>31</v>
       </c>
       <c r="J33" s="1"/>
-      <c r="M33" s="7"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="6"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>24</v>
       </c>
@@ -1380,7 +1492,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>36</v>
       </c>
@@ -1398,7 +1510,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>48</v>
       </c>
@@ -1413,7 +1525,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>12</v>
       </c>
@@ -1428,7 +1540,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>28</v>
       </c>
@@ -1448,7 +1560,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>29</v>
       </c>
@@ -1468,7 +1580,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>30</v>
       </c>
@@ -1485,7 +1597,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>31</v>
       </c>
@@ -1511,4 +1623,141 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>